<commit_message>
feat:produced scatter chart for probabilities
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/sample_0/category__0.xlsx
+++ b/06-03-2023/data/output/xlsx/sample_0/category__0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="131">
   <si>
     <t>Causality Values Chart</t>
   </si>
@@ -61,6 +61,30 @@
     <t>n/a</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__3</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__4</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__5</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__6</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__7</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__8</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__9</t>
+  </si>
+  <si>
     <t>num_of_adds_and_subs__10</t>
   </si>
   <si>
@@ -88,28 +112,139 @@
     <t>num_of_adds_and_subs__18</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__2</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__4</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__5</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__6</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__7</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__8</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__9</t>
+    <t>num_of_mults_and_divs__0</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__1</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__2</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__3</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__4</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__5</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__6</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__7</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__8</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__9</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__10</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__11</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__12</t>
+  </si>
+  <si>
+    <t>num_of_mults_and_divs__13</t>
+  </si>
+  <si>
+    <t>num_of_equals__0</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_equals__1</t>
+  </si>
+  <si>
+    <t>num_of_equals__1</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_equals__0</t>
+  </si>
+  <si>
+    <t>num_of_equals__2</t>
+  </si>
+  <si>
+    <t>num_of_equals__3</t>
+  </si>
+  <si>
+    <t>num_of_equals__4</t>
+  </si>
+  <si>
+    <t>num_of_equals__5</t>
+  </si>
+  <si>
+    <t>num_of_equals__6</t>
+  </si>
+  <si>
+    <t>num_of_equals__7</t>
+  </si>
+  <si>
+    <t>num_of_equals__8</t>
+  </si>
+  <si>
+    <t>num_of_equals__9</t>
+  </si>
+  <si>
+    <t>num_of_equals__10</t>
+  </si>
+  <si>
+    <t>num_of_equals__11</t>
+  </si>
+  <si>
+    <t>num_of_equals__12</t>
+  </si>
+  <si>
+    <t>num_of_equals__13</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__0</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__1</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__3</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__4</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__5</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__6</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__7</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__8</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__9</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__10</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__11</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__12</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__13</t>
+  </si>
+  <si>
+    <t>pairs_of_parentheses__14</t>
   </si>
   <si>
     <t>num_of_decimals__0</t>
@@ -118,6 +253,30 @@
     <t>num_of_decimals__1</t>
   </si>
   <si>
+    <t>num_of_decimals__2</t>
+  </si>
+  <si>
+    <t>num_of_decimals__3</t>
+  </si>
+  <si>
+    <t>num_of_decimals__4</t>
+  </si>
+  <si>
+    <t>num_of_decimals__5</t>
+  </si>
+  <si>
+    <t>num_of_decimals__6</t>
+  </si>
+  <si>
+    <t>num_of_decimals__7</t>
+  </si>
+  <si>
+    <t>num_of_decimals__8</t>
+  </si>
+  <si>
+    <t>num_of_decimals__9</t>
+  </si>
+  <si>
     <t>num_of_decimals__10</t>
   </si>
   <si>
@@ -148,9 +307,6 @@
     <t>num_of_decimals__19</t>
   </si>
   <si>
-    <t>num_of_decimals__2</t>
-  </si>
-  <si>
     <t>num_of_decimals__20</t>
   </si>
   <si>
@@ -181,123 +337,36 @@
     <t>num_of_decimals__29</t>
   </si>
   <si>
-    <t>num_of_decimals__3</t>
-  </si>
-  <si>
-    <t>num_of_decimals__4</t>
-  </si>
-  <si>
-    <t>num_of_decimals__5</t>
-  </si>
-  <si>
-    <t>num_of_decimals__6</t>
-  </si>
-  <si>
-    <t>num_of_decimals__7</t>
-  </si>
-  <si>
-    <t>num_of_decimals__8</t>
-  </si>
-  <si>
-    <t>num_of_decimals__9</t>
-  </si>
-  <si>
-    <t>num_of_equals__0</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_equals__1</t>
-  </si>
-  <si>
-    <t>num_of_equals__1</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_equals__0</t>
-  </si>
-  <si>
-    <t>num_of_equals__10</t>
-  </si>
-  <si>
-    <t>num_of_equals__11</t>
-  </si>
-  <si>
-    <t>num_of_equals__12</t>
-  </si>
-  <si>
-    <t>num_of_equals__13</t>
-  </si>
-  <si>
-    <t>num_of_equals__2</t>
-  </si>
-  <si>
-    <t>num_of_equals__3</t>
-  </si>
-  <si>
-    <t>num_of_equals__4</t>
-  </si>
-  <si>
-    <t>num_of_equals__5</t>
-  </si>
-  <si>
-    <t>num_of_equals__6</t>
-  </si>
-  <si>
-    <t>num_of_equals__7</t>
-  </si>
-  <si>
-    <t>num_of_equals__8</t>
-  </si>
-  <si>
-    <t>num_of_equals__9</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__0</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__1</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__10</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__11</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__12</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__13</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__2</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__3</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__4</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__5</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__6</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__7</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__8</t>
-  </si>
-  <si>
-    <t>num_of_mults_and_divs__9</t>
-  </si>
-  <si>
     <t>num_of_unknowns__0</t>
   </si>
   <si>
     <t>num_of_unknowns__1</t>
   </si>
   <si>
+    <t>num_of_unknowns__2</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__3</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__4</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__5</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__6</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__7</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__8</t>
+  </si>
+  <si>
+    <t>num_of_unknowns__9</t>
+  </si>
+  <si>
     <t>num_of_unknowns__10</t>
   </si>
   <si>
@@ -305,75 +374,6 @@
   </si>
   <si>
     <t>num_of_unknowns__12</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__2</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__3</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__4</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__5</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__6</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__7</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__8</t>
-  </si>
-  <si>
-    <t>num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__0</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__1</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__10</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__11</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__12</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__13</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__14</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__2</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__3</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__4</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__5</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__6</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__7</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__8</t>
-  </si>
-  <si>
-    <t>pairs_of_parentheses__9</t>
   </si>
   <si>
     <t>Number of Additions And Subtractions Chart</t>
@@ -529,30 +529,78 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>AddsSubs!$C$4:$C$7</c:f>
+              <c:f>AddsSubs!$C$4:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>AddsSubs!$D$4:$D$7</c:f>
+              <c:f>AddsSubs!$D$4:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.5137895812053116</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5036319612590799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4336569579288026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3686868686868687</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3164556962025317</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.275</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1363636363636364</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,10 +721,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>MultsDivs!$C$4:$C$9</c:f>
+              <c:f>MultsDivs!$C$4:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -688,16 +736,40 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MultsDivs!$D$4:$D$9</c:f>
+              <c:f>MultsDivs!$D$4:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.3796791443850268</c:v>
                 </c:pt>
@@ -705,9 +777,33 @@
                   <c:v>0.3802816901408451</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3287671232876712</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3148148148148148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2702702702702703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2941176470588235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4545454545454545</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>0.3333333333333333</c:v>
                 </c:pt>
               </c:numCache>
@@ -829,30 +925,78 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Equations!$C$4:$C$7</c:f>
+              <c:f>Equations!$C$4:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Equations!$D$4:$D$7</c:f>
+              <c:f>Equations!$D$4:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.5125376128385155</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5146316851664985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4860853432282004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4302325581395349</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.357843137254902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3161764705882353</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3260869565217391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3518518518518519</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.05882352941176471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -973,10 +1117,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Decimals!$C$4:$C$10</c:f>
+              <c:f>Decimals!$C$4:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -991,16 +1135,40 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Decimals!$D$4:$D$10</c:f>
+              <c:f>Decimals!$D$4:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0.4196141479099679</c:v>
                 </c:pt>
@@ -1008,12 +1176,36 @@
                   <c:v>0.3678861788617886</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.3424657534246575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2806324110671937</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2754491017964072</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.246031746031746</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2153846153846154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1951219512195122</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1612903225806452</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.2173913043478261</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1135,30 +1327,72 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Unknowns!$C$4:$C$7</c:f>
+              <c:f>Unknowns!$C$4:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Unknowns!$D$4:$D$7</c:f>
+              <c:f>Unknowns!$D$4:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.5120240480961924</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.4904831625183016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2842105263157895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2608695652173913</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3636363636363636</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,30 +1513,54 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>PairsOfParentheses!$C$4:$C$7</c:f>
+              <c:f>PairsOfParentheses!$C$4:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PairsOfParentheses!$D$4:$D$7</c:f>
+              <c:f>PairsOfParentheses!$D$4:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.449748743718593</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.3121019108280255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2558139534883721</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1764705882352941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1963,13 +2221,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>309</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>0.4336569579288026</v>
       </c>
       <c r="E5" s="1">
         <v>0.5120240480961924</v>
@@ -1984,13 +2242,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>198</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>0.3686868686868687</v>
       </c>
       <c r="E6" s="1">
         <v>0.5120240480961924</v>
@@ -2005,13 +2263,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="E7" s="1">
         <v>0.5120240480961924</v>
@@ -2026,13 +2284,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>0.3164556962025317</v>
       </c>
       <c r="E8" s="1">
         <v>0.5120240480961924</v>
@@ -2047,13 +2305,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>0.2692307692307692</v>
       </c>
       <c r="E9" s="1">
         <v>0.5120240480961924</v>
@@ -2068,13 +2326,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>0.275</v>
       </c>
       <c r="E10" s="1">
         <v>0.5120240480961924</v>
@@ -2089,13 +2347,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>0.1363636363636364</v>
       </c>
       <c r="E11" s="1">
         <v>0.5120240480961924</v>
@@ -2110,13 +2368,13 @@
         <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E12" s="1">
         <v>0.5120240480961924</v>
@@ -2131,7 +2389,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>11</v>
@@ -2152,13 +2410,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>309</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>12</v>
       </c>
       <c r="D14" s="1">
-        <v>0.4336569579288026</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0.5120240480961924</v>
@@ -2173,13 +2431,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>198</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1">
         <v>13</v>
       </c>
       <c r="D15" s="1">
-        <v>0.3686868686868687</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>0.5120240480961924</v>
@@ -2194,13 +2452,13 @@
         <v>24</v>
       </c>
       <c r="B16" s="1">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1">
         <v>14</v>
       </c>
       <c r="D16" s="1">
-        <v>0.3142857142857143</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>0.5120240480961924</v>
@@ -2215,13 +2473,13 @@
         <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>15</v>
       </c>
       <c r="D17" s="1">
-        <v>0.3164556962025317</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>0.5120240480961924</v>
@@ -2236,13 +2494,13 @@
         <v>26</v>
       </c>
       <c r="B18" s="1">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1">
         <v>16</v>
       </c>
       <c r="D18" s="1">
-        <v>0.2692307692307692</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>0.5120240480961924</v>
@@ -2257,13 +2515,13 @@
         <v>27</v>
       </c>
       <c r="B19" s="1">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1">
         <v>17</v>
       </c>
       <c r="D19" s="1">
-        <v>0.275</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
         <v>0.5120240480961924</v>
@@ -2278,13 +2536,13 @@
         <v>28</v>
       </c>
       <c r="B20" s="1">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1">
         <v>18</v>
       </c>
       <c r="D20" s="1">
-        <v>0.1363636363636364</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>0.5120240480961924</v>
@@ -2299,13 +2557,13 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1">
         <v>19</v>
       </c>
       <c r="D21" s="1">
-        <v>0.1111111111111111</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
         <v>0.5120240480961924</v>
@@ -2320,13 +2578,13 @@
         <v>30</v>
       </c>
       <c r="B22" s="1">
-        <v>622</v>
+        <v>187</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
       </c>
       <c r="D22" s="1">
-        <v>0.4196141479099679</v>
+        <v>0.3796791443850268</v>
       </c>
       <c r="E22" s="1">
         <v>0.5120240480961924</v>
@@ -2341,13 +2599,13 @@
         <v>31</v>
       </c>
       <c r="B23" s="1">
-        <v>492</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1">
         <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>0.3678861788617886</v>
+        <v>0.3802816901408451</v>
       </c>
       <c r="E23" s="1">
         <v>0.5120240480961924</v>
@@ -2362,13 +2620,13 @@
         <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1">
         <v>22</v>
       </c>
       <c r="D24" s="1">
-        <v>0.2173913043478261</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E24" s="1">
         <v>0.5120240480961924</v>
@@ -2383,13 +2641,13 @@
         <v>33</v>
       </c>
       <c r="B25" s="1">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1">
         <v>23</v>
       </c>
       <c r="D25" s="1">
-        <v>0.2</v>
+        <v>0.3287671232876712</v>
       </c>
       <c r="E25" s="1">
         <v>0.5120240480961924</v>
@@ -2404,13 +2662,13 @@
         <v>34</v>
       </c>
       <c r="B26" s="1">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1">
         <v>24</v>
       </c>
       <c r="D26" s="1">
-        <v>0.1</v>
+        <v>0.3148148148148148</v>
       </c>
       <c r="E26" s="1">
         <v>0.5120240480961924</v>
@@ -2425,13 +2683,13 @@
         <v>35</v>
       </c>
       <c r="B27" s="1">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
         <v>25</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.2702702702702703</v>
       </c>
       <c r="E27" s="1">
         <v>0.5120240480961924</v>
@@ -2446,13 +2704,13 @@
         <v>36</v>
       </c>
       <c r="B28" s="1">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1">
         <v>26</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.3181818181818182</v>
       </c>
       <c r="E28" s="1">
         <v>0.5120240480961924</v>
@@ -2467,13 +2725,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1">
         <v>27</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="E29" s="1">
         <v>0.5120240480961924</v>
@@ -2488,13 +2746,13 @@
         <v>38</v>
       </c>
       <c r="B30" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1">
         <v>28</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="E30" s="1">
         <v>0.5120240480961924</v>
@@ -2509,13 +2767,13 @@
         <v>39</v>
       </c>
       <c r="B31" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1">
         <v>29</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E31" s="1">
         <v>0.5120240480961924</v>
@@ -2530,13 +2788,13 @@
         <v>40</v>
       </c>
       <c r="B32" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
         <v>30</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E32" s="1">
         <v>0.5120240480961924</v>
@@ -2557,7 +2815,7 @@
         <v>31</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E33" s="1">
         <v>0.5120240480961924</v>
@@ -2572,13 +2830,13 @@
         <v>42</v>
       </c>
       <c r="B34" s="1">
-        <v>365</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1">
         <v>32</v>
       </c>
       <c r="D34" s="1">
-        <v>0.3424657534246575</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
         <v>0.5120240480961924</v>
@@ -2593,7 +2851,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="1">
         <v>33</v>
@@ -2614,55 +2872,59 @@
         <v>44</v>
       </c>
       <c r="B36" s="1">
-        <v>2</v>
+        <v>997</v>
       </c>
       <c r="C36" s="1">
         <v>34</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>0.5125376128385155</v>
       </c>
       <c r="E36" s="1">
         <v>0.5120240480961924</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
-        <v>12</v>
+      <c r="F36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.5144733067959282</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1">
-        <v>2</v>
+        <v>991</v>
       </c>
       <c r="C37" s="1">
         <v>35</v>
       </c>
       <c r="D37" s="1">
-        <v>0</v>
+        <v>0.5146316851664985</v>
       </c>
       <c r="E37" s="1">
         <v>0.5120240480961924</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>12</v>
+      <c r="F37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.3607843904962417</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1">
-        <v>2</v>
+        <v>539</v>
       </c>
       <c r="C38" s="1">
         <v>36</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>0.4860853432282004</v>
       </c>
       <c r="E38" s="1">
         <v>0.5120240480961924</v>
@@ -2674,16 +2936,16 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <v>344</v>
       </c>
       <c r="C39" s="1">
         <v>37</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>0.4302325581395349</v>
       </c>
       <c r="E39" s="1">
         <v>0.5120240480961924</v>
@@ -2695,16 +2957,16 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="C40" s="1">
         <v>38</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>0.357843137254902</v>
       </c>
       <c r="E40" s="1">
         <v>0.5120240480961924</v>
@@ -2716,16 +2978,16 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="C41" s="1">
         <v>39</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>0.3161764705882353</v>
       </c>
       <c r="E41" s="1">
         <v>0.5120240480961924</v>
@@ -2737,16 +2999,16 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B42" s="1">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1">
         <v>40</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>0.3260869565217391</v>
       </c>
       <c r="E42" s="1">
         <v>0.5120240480961924</v>
@@ -2758,16 +3020,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B43" s="1">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C43" s="1">
         <v>41</v>
       </c>
       <c r="D43" s="1">
-        <v>0</v>
+        <v>0.3518518518518519</v>
       </c>
       <c r="E43" s="1">
         <v>0.5120240480961924</v>
@@ -2779,16 +3041,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B44" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C44" s="1">
         <v>42</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>0.3428571428571429</v>
       </c>
       <c r="E44" s="1">
         <v>0.5120240480961924</v>
@@ -2800,16 +3062,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1">
-        <v>253</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1">
         <v>43</v>
       </c>
       <c r="D45" s="1">
-        <v>0.2806324110671937</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="E45" s="1">
         <v>0.5120240480961924</v>
@@ -2821,16 +3083,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B46" s="1">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="C46" s="1">
         <v>44</v>
       </c>
       <c r="D46" s="1">
-        <v>0.2754491017964072</v>
+        <v>0</v>
       </c>
       <c r="E46" s="1">
         <v>0.5120240480961924</v>
@@ -2842,16 +3104,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1">
         <v>45</v>
       </c>
       <c r="D47" s="1">
-        <v>0.246031746031746</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
         <v>0.5120240480961924</v>
@@ -2863,16 +3125,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C48" s="1">
         <v>46</v>
       </c>
       <c r="D48" s="1">
-        <v>0.1882352941176471</v>
+        <v>0</v>
       </c>
       <c r="E48" s="1">
         <v>0.5120240480961924</v>
@@ -2884,16 +3146,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="C49" s="1">
         <v>47</v>
       </c>
       <c r="D49" s="1">
-        <v>0.2153846153846154</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
         <v>0.5120240480961924</v>
@@ -2905,16 +3167,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1">
-        <v>41</v>
+        <v>398</v>
       </c>
       <c r="C50" s="1">
         <v>48</v>
       </c>
       <c r="D50" s="1">
-        <v>0.1951219512195122</v>
+        <v>0.449748743718593</v>
       </c>
       <c r="E50" s="1">
         <v>0.5120240480961924</v>
@@ -2926,16 +3188,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="C51" s="1">
         <v>49</v>
       </c>
       <c r="D51" s="1">
-        <v>0.1612903225806452</v>
+        <v>0.3121019108280255</v>
       </c>
       <c r="E51" s="1">
         <v>0.5120240480961924</v>
@@ -2947,48 +3209,44 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1">
-        <v>997</v>
+        <v>75</v>
       </c>
       <c r="C52" s="1">
         <v>50</v>
       </c>
       <c r="D52" s="1">
-        <v>0.5125376128385155</v>
+        <v>0.32</v>
       </c>
       <c r="E52" s="1">
         <v>0.5120240480961924</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G52" s="1">
-        <v>0.5144733067959282</v>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1">
-        <v>991</v>
+        <v>43</v>
       </c>
       <c r="C53" s="1">
         <v>51</v>
       </c>
       <c r="D53" s="1">
-        <v>0.5146316851664985</v>
+        <v>0.2558139534883721</v>
       </c>
       <c r="E53" s="1">
         <v>0.5120240480961924</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0.3607843904962417</v>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2996,13 +3254,13 @@
         <v>64</v>
       </c>
       <c r="B54" s="1">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C54" s="1">
         <v>52</v>
       </c>
       <c r="D54" s="1">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="E54" s="1">
         <v>0.5120240480961924</v>
@@ -3017,13 +3275,13 @@
         <v>65</v>
       </c>
       <c r="B55" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1">
         <v>53</v>
       </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="E55" s="1">
         <v>0.5120240480961924</v>
@@ -3038,7 +3296,7 @@
         <v>66</v>
       </c>
       <c r="B56" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1">
         <v>54</v>
@@ -3059,7 +3317,7 @@
         <v>67</v>
       </c>
       <c r="B57" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C57" s="1">
         <v>55</v>
@@ -3080,13 +3338,13 @@
         <v>68</v>
       </c>
       <c r="B58" s="1">
-        <v>539</v>
+        <v>3</v>
       </c>
       <c r="C58" s="1">
         <v>56</v>
       </c>
       <c r="D58" s="1">
-        <v>0.4860853432282004</v>
+        <v>0</v>
       </c>
       <c r="E58" s="1">
         <v>0.5120240480961924</v>
@@ -3101,13 +3359,13 @@
         <v>69</v>
       </c>
       <c r="B59" s="1">
-        <v>344</v>
+        <v>3</v>
       </c>
       <c r="C59" s="1">
         <v>57</v>
       </c>
       <c r="D59" s="1">
-        <v>0.4302325581395349</v>
+        <v>0</v>
       </c>
       <c r="E59" s="1">
         <v>0.5120240480961924</v>
@@ -3122,13 +3380,13 @@
         <v>70</v>
       </c>
       <c r="B60" s="1">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="C60" s="1">
         <v>58</v>
       </c>
       <c r="D60" s="1">
-        <v>0.357843137254902</v>
+        <v>0</v>
       </c>
       <c r="E60" s="1">
         <v>0.5120240480961924</v>
@@ -3143,13 +3401,13 @@
         <v>71</v>
       </c>
       <c r="B61" s="1">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="C61" s="1">
         <v>59</v>
       </c>
       <c r="D61" s="1">
-        <v>0.3161764705882353</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1">
         <v>0.5120240480961924</v>
@@ -3164,13 +3422,13 @@
         <v>72</v>
       </c>
       <c r="B62" s="1">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C62" s="1">
         <v>60</v>
       </c>
       <c r="D62" s="1">
-        <v>0.3260869565217391</v>
+        <v>0</v>
       </c>
       <c r="E62" s="1">
         <v>0.5120240480961924</v>
@@ -3185,13 +3443,13 @@
         <v>73</v>
       </c>
       <c r="B63" s="1">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C63" s="1">
         <v>61</v>
       </c>
       <c r="D63" s="1">
-        <v>0.3518518518518519</v>
+        <v>0</v>
       </c>
       <c r="E63" s="1">
         <v>0.5120240480961924</v>
@@ -3206,13 +3464,13 @@
         <v>74</v>
       </c>
       <c r="B64" s="1">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C64" s="1">
         <v>62</v>
       </c>
       <c r="D64" s="1">
-        <v>0.3428571428571429</v>
+        <v>0</v>
       </c>
       <c r="E64" s="1">
         <v>0.5120240480961924</v>
@@ -3227,13 +3485,13 @@
         <v>75</v>
       </c>
       <c r="B65" s="1">
-        <v>17</v>
+        <v>622</v>
       </c>
       <c r="C65" s="1">
         <v>63</v>
       </c>
       <c r="D65" s="1">
-        <v>0.05882352941176471</v>
+        <v>0.4196141479099679</v>
       </c>
       <c r="E65" s="1">
         <v>0.5120240480961924</v>
@@ -3248,13 +3506,13 @@
         <v>76</v>
       </c>
       <c r="B66" s="1">
-        <v>187</v>
+        <v>492</v>
       </c>
       <c r="C66" s="1">
         <v>64</v>
       </c>
       <c r="D66" s="1">
-        <v>0.3796791443850268</v>
+        <v>0.3678861788617886</v>
       </c>
       <c r="E66" s="1">
         <v>0.5120240480961924</v>
@@ -3269,13 +3527,13 @@
         <v>77</v>
       </c>
       <c r="B67" s="1">
-        <v>142</v>
+        <v>365</v>
       </c>
       <c r="C67" s="1">
         <v>65</v>
       </c>
       <c r="D67" s="1">
-        <v>0.3802816901408451</v>
+        <v>0.3424657534246575</v>
       </c>
       <c r="E67" s="1">
         <v>0.5120240480961924</v>
@@ -3290,13 +3548,13 @@
         <v>78</v>
       </c>
       <c r="B68" s="1">
-        <v>5</v>
+        <v>253</v>
       </c>
       <c r="C68" s="1">
         <v>66</v>
       </c>
       <c r="D68" s="1">
-        <v>0.4</v>
+        <v>0.2806324110671937</v>
       </c>
       <c r="E68" s="1">
         <v>0.5120240480961924</v>
@@ -3311,13 +3569,13 @@
         <v>79</v>
       </c>
       <c r="B69" s="1">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="C69" s="1">
         <v>67</v>
       </c>
       <c r="D69" s="1">
-        <v>0.3333333333333333</v>
+        <v>0.2754491017964072</v>
       </c>
       <c r="E69" s="1">
         <v>0.5120240480961924</v>
@@ -3332,13 +3590,13 @@
         <v>80</v>
       </c>
       <c r="B70" s="1">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="C70" s="1">
         <v>68</v>
       </c>
       <c r="D70" s="1">
-        <v>0</v>
+        <v>0.246031746031746</v>
       </c>
       <c r="E70" s="1">
         <v>0.5120240480961924</v>
@@ -3353,13 +3611,13 @@
         <v>81</v>
       </c>
       <c r="B71" s="1">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C71" s="1">
         <v>69</v>
       </c>
       <c r="D71" s="1">
-        <v>0</v>
+        <v>0.1882352941176471</v>
       </c>
       <c r="E71" s="1">
         <v>0.5120240480961924</v>
@@ -3374,13 +3632,13 @@
         <v>82</v>
       </c>
       <c r="B72" s="1">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C72" s="1">
         <v>70</v>
       </c>
       <c r="D72" s="1">
-        <v>0.3333333333333333</v>
+        <v>0.2153846153846154</v>
       </c>
       <c r="E72" s="1">
         <v>0.5120240480961924</v>
@@ -3395,13 +3653,13 @@
         <v>83</v>
       </c>
       <c r="B73" s="1">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C73" s="1">
         <v>71</v>
       </c>
       <c r="D73" s="1">
-        <v>0.3287671232876712</v>
+        <v>0.1951219512195122</v>
       </c>
       <c r="E73" s="1">
         <v>0.5120240480961924</v>
@@ -3416,13 +3674,13 @@
         <v>84</v>
       </c>
       <c r="B74" s="1">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C74" s="1">
         <v>72</v>
       </c>
       <c r="D74" s="1">
-        <v>0.3148148148148148</v>
+        <v>0.1612903225806452</v>
       </c>
       <c r="E74" s="1">
         <v>0.5120240480961924</v>
@@ -3437,13 +3695,13 @@
         <v>85</v>
       </c>
       <c r="B75" s="1">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C75" s="1">
         <v>73</v>
       </c>
       <c r="D75" s="1">
-        <v>0.2702702702702703</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="E75" s="1">
         <v>0.5120240480961924</v>
@@ -3458,13 +3716,13 @@
         <v>86</v>
       </c>
       <c r="B76" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C76" s="1">
         <v>74</v>
       </c>
       <c r="D76" s="1">
-        <v>0.3181818181818182</v>
+        <v>0.2</v>
       </c>
       <c r="E76" s="1">
         <v>0.5120240480961924</v>
@@ -3479,13 +3737,13 @@
         <v>87</v>
       </c>
       <c r="B77" s="1">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1">
         <v>75</v>
       </c>
       <c r="D77" s="1">
-        <v>0.2941176470588235</v>
+        <v>0.1</v>
       </c>
       <c r="E77" s="1">
         <v>0.5120240480961924</v>
@@ -3500,13 +3758,13 @@
         <v>88</v>
       </c>
       <c r="B78" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1">
         <v>76</v>
       </c>
       <c r="D78" s="1">
-        <v>0.4545454545454545</v>
+        <v>0</v>
       </c>
       <c r="E78" s="1">
         <v>0.5120240480961924</v>
@@ -3521,13 +3779,13 @@
         <v>89</v>
       </c>
       <c r="B79" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C79" s="1">
         <v>77</v>
       </c>
       <c r="D79" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E79" s="1">
         <v>0.5120240480961924</v>
@@ -3542,13 +3800,13 @@
         <v>90</v>
       </c>
       <c r="B80" s="1">
-        <v>998</v>
+        <v>6</v>
       </c>
       <c r="C80" s="1">
         <v>78</v>
       </c>
       <c r="D80" s="1">
-        <v>0.5120240480961924</v>
+        <v>0</v>
       </c>
       <c r="E80" s="1">
         <v>0.5120240480961924</v>
@@ -3563,13 +3821,13 @@
         <v>91</v>
       </c>
       <c r="B81" s="1">
-        <v>683</v>
+        <v>5</v>
       </c>
       <c r="C81" s="1">
         <v>79</v>
       </c>
       <c r="D81" s="1">
-        <v>0.4904831625183016</v>
+        <v>0</v>
       </c>
       <c r="E81" s="1">
         <v>0.5120240480961924</v>
@@ -3584,7 +3842,7 @@
         <v>92</v>
       </c>
       <c r="B82" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C82" s="1">
         <v>80</v>
@@ -3605,7 +3863,7 @@
         <v>93</v>
       </c>
       <c r="B83" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C83" s="1">
         <v>81</v>
@@ -3626,7 +3884,7 @@
         <v>94</v>
       </c>
       <c r="B84" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C84" s="1">
         <v>82</v>
@@ -3647,13 +3905,13 @@
         <v>95</v>
       </c>
       <c r="B85" s="1">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="C85" s="1">
         <v>83</v>
       </c>
       <c r="D85" s="1">
-        <v>0.2842105263157895</v>
+        <v>0</v>
       </c>
       <c r="E85" s="1">
         <v>0.5120240480961924</v>
@@ -3668,13 +3926,13 @@
         <v>96</v>
       </c>
       <c r="B86" s="1">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C86" s="1">
         <v>84</v>
       </c>
       <c r="D86" s="1">
-        <v>0.1923076923076923</v>
+        <v>0</v>
       </c>
       <c r="E86" s="1">
         <v>0.5120240480961924</v>
@@ -3689,13 +3947,13 @@
         <v>97</v>
       </c>
       <c r="B87" s="1">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C87" s="1">
         <v>85</v>
       </c>
       <c r="D87" s="1">
-        <v>0.2608695652173913</v>
+        <v>0</v>
       </c>
       <c r="E87" s="1">
         <v>0.5120240480961924</v>
@@ -3710,13 +3968,13 @@
         <v>98</v>
       </c>
       <c r="B88" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C88" s="1">
         <v>86</v>
       </c>
       <c r="D88" s="1">
-        <v>0.2857142857142857</v>
+        <v>0</v>
       </c>
       <c r="E88" s="1">
         <v>0.5120240480961924</v>
@@ -3731,13 +3989,13 @@
         <v>99</v>
       </c>
       <c r="B89" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C89" s="1">
         <v>87</v>
       </c>
       <c r="D89" s="1">
-        <v>0.3636363636363636</v>
+        <v>0</v>
       </c>
       <c r="E89" s="1">
         <v>0.5120240480961924</v>
@@ -3752,13 +4010,13 @@
         <v>100</v>
       </c>
       <c r="B90" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C90" s="1">
         <v>88</v>
       </c>
       <c r="D90" s="1">
-        <v>0.2857142857142857</v>
+        <v>0</v>
       </c>
       <c r="E90" s="1">
         <v>0.5120240480961924</v>
@@ -3773,13 +4031,13 @@
         <v>101</v>
       </c>
       <c r="B91" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C91" s="1">
         <v>89</v>
       </c>
       <c r="D91" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E91" s="1">
         <v>0.5120240480961924</v>
@@ -3794,7 +4052,7 @@
         <v>102</v>
       </c>
       <c r="B92" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1">
         <v>90</v>
@@ -3815,13 +4073,13 @@
         <v>103</v>
       </c>
       <c r="B93" s="1">
-        <v>398</v>
+        <v>1</v>
       </c>
       <c r="C93" s="1">
         <v>91</v>
       </c>
       <c r="D93" s="1">
-        <v>0.449748743718593</v>
+        <v>0</v>
       </c>
       <c r="E93" s="1">
         <v>0.5120240480961924</v>
@@ -3836,13 +4094,13 @@
         <v>104</v>
       </c>
       <c r="B94" s="1">
-        <v>157</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1">
         <v>92</v>
       </c>
       <c r="D94" s="1">
-        <v>0.3121019108280255</v>
+        <v>0</v>
       </c>
       <c r="E94" s="1">
         <v>0.5120240480961924</v>
@@ -3857,13 +4115,13 @@
         <v>105</v>
       </c>
       <c r="B95" s="1">
-        <v>3</v>
+        <v>998</v>
       </c>
       <c r="C95" s="1">
         <v>93</v>
       </c>
       <c r="D95" s="1">
-        <v>0</v>
+        <v>0.5120240480961924</v>
       </c>
       <c r="E95" s="1">
         <v>0.5120240480961924</v>
@@ -3878,13 +4136,13 @@
         <v>106</v>
       </c>
       <c r="B96" s="1">
-        <v>3</v>
+        <v>683</v>
       </c>
       <c r="C96" s="1">
         <v>94</v>
       </c>
       <c r="D96" s="1">
-        <v>0</v>
+        <v>0.4904831625183016</v>
       </c>
       <c r="E96" s="1">
         <v>0.5120240480961924</v>
@@ -3899,13 +4157,13 @@
         <v>107</v>
       </c>
       <c r="B97" s="1">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C97" s="1">
         <v>95</v>
       </c>
       <c r="D97" s="1">
-        <v>0</v>
+        <v>0.2842105263157895</v>
       </c>
       <c r="E97" s="1">
         <v>0.5120240480961924</v>
@@ -3920,13 +4178,13 @@
         <v>108</v>
       </c>
       <c r="B98" s="1">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C98" s="1">
         <v>96</v>
       </c>
       <c r="D98" s="1">
-        <v>0</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="E98" s="1">
         <v>0.5120240480961924</v>
@@ -3941,13 +4199,13 @@
         <v>109</v>
       </c>
       <c r="B99" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C99" s="1">
         <v>97</v>
       </c>
       <c r="D99" s="1">
-        <v>0</v>
+        <v>0.2608695652173913</v>
       </c>
       <c r="E99" s="1">
         <v>0.5120240480961924</v>
@@ -3962,13 +4220,13 @@
         <v>110</v>
       </c>
       <c r="B100" s="1">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C100" s="1">
         <v>98</v>
       </c>
       <c r="D100" s="1">
-        <v>0.32</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E100" s="1">
         <v>0.5120240480961924</v>
@@ -3983,13 +4241,13 @@
         <v>111</v>
       </c>
       <c r="B101" s="1">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="C101" s="1">
         <v>99</v>
       </c>
       <c r="D101" s="1">
-        <v>0.2558139534883721</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="E101" s="1">
         <v>0.5120240480961924</v>
@@ -4004,13 +4262,13 @@
         <v>112</v>
       </c>
       <c r="B102" s="1">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C102" s="1">
         <v>100</v>
       </c>
       <c r="D102" s="1">
-        <v>0.16</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E102" s="1">
         <v>0.5120240480961924</v>
@@ -4025,13 +4283,13 @@
         <v>113</v>
       </c>
       <c r="B103" s="1">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C103" s="1">
         <v>101</v>
       </c>
       <c r="D103" s="1">
-        <v>0.1764705882352941</v>
+        <v>0.4</v>
       </c>
       <c r="E103" s="1">
         <v>0.5120240480961924</v>
@@ -4046,7 +4304,7 @@
         <v>114</v>
       </c>
       <c r="B104" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C104" s="1">
         <v>102</v>
@@ -4067,7 +4325,7 @@
         <v>115</v>
       </c>
       <c r="B105" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C105" s="1">
         <v>103</v>
@@ -4088,7 +4346,7 @@
         <v>116</v>
       </c>
       <c r="B106" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C106" s="1">
         <v>104</v>
@@ -4109,7 +4367,7 @@
         <v>117</v>
       </c>
       <c r="B107" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C107" s="1">
         <v>105</v>
@@ -4132,7 +4390,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4273,6 +4531,350 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>309</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.4336569579288026</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.0783670901673898</v>
+      </c>
+      <c r="G6" s="1">
+        <f>1/(POWER(B6,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>G6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MIN(K6,1-D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>198</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.3686868686868687</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-0.1433371794093237</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1/(POWER(B7,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SQRT((D7-POWER(10,-4))*B7*((1-D7+POWER(10,-4))*B7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>105</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.3142857142857143</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.1977383338104781</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>79</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.3164556962025317</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.1955683518936607</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.2692307692307692</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.2427932788654232</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.275</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.2370240480961924</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.1363636363636364</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.375660411732556</v>
+      </c>
+      <c r="G12" s="1">
+        <f>1/(POWER(B12,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SQRT((D12-POWER(10,-4))*B12*((1-D12+POWER(10,-4))*B12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K12" s="1">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(K12,1-D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.4009129369850813</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1/(POWER(B13,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f>SQRT((D13-POWER(10,-4))*B13*((1-D13+POWER(10,-4))*B13))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K13" s="1">
+        <f>I13*J13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(K13,1-D13)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4281,7 +4883,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4338,7 +4940,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3">
         <v>187</v>
@@ -4381,7 +4983,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>142</v>
@@ -4424,22 +5026,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>0.4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E6" s="3">
         <v>0.5120240480961924</v>
       </c>
       <c r="F6" s="1">
-        <v>-0.1120240480961924</v>
+        <v>-0.1786907147628591</v>
       </c>
       <c r="G6" s="1">
         <f>1/(POWER(B6,1.5))</f>
@@ -4467,22 +5069,22 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="3">
-        <v>0.3333333333333333</v>
+        <v>0.3287671232876712</v>
       </c>
       <c r="E7" s="3">
         <v>0.5120240480961924</v>
       </c>
       <c r="F7" s="1">
-        <v>-0.1786907147628591</v>
+        <v>-0.1832569248085212</v>
       </c>
       <c r="G7" s="1">
         <f>1/(POWER(B7,1.5))</f>
@@ -4505,6 +5107,350 @@
       </c>
       <c r="L7" s="1">
         <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.3148148148148148</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.1972092332813776</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.2702702702702703</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.2417537778259221</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.3181818181818182</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.1938422299143742</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.2941176470588235</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.2179064010373689</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.05747859355073787</v>
+      </c>
+      <c r="G12" s="1">
+        <f>1/(POWER(B12,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SQRT((D12-POWER(10,-4))*B12*((1-D12+POWER(10,-4))*B12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K12" s="1">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(K12,1-D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.2620240480961924</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1/(POWER(B13,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f>SQRT((D13-POWER(10,-4))*B13*((1-D13+POWER(10,-4))*B13))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K13" s="1">
+        <f>I13*J13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(K13,1-D13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.1120240480961924</v>
+      </c>
+      <c r="G14" s="1">
+        <f>1/(POWER(B14,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f>SQRT((D14-POWER(10,-4))*B14*((1-D14+POWER(10,-4))*B14))</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f>G14*H14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14*J14</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(K14,1-D14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-0.1786907147628591</v>
+      </c>
+      <c r="G15" s="1">
+        <f>1/(POWER(B15,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SQRT((D15-POWER(10,-4))*B15*((1-D15+POWER(10,-4))*B15))</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f>G15*H15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K15" s="1">
+        <f>I15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(K15,1-D15)</f>
         <v>0</v>
       </c>
     </row>
@@ -4516,7 +5462,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4573,7 +5519,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3">
         <v>997</v>
@@ -4616,7 +5562,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3">
         <v>991</v>
@@ -4654,6 +5600,350 @@
       </c>
       <c r="L5" s="1">
         <f>MIN(K5,1-D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3">
+        <v>539</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.4860853432282004</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.02593870486799205</v>
+      </c>
+      <c r="G6" s="1">
+        <f>1/(POWER(B6,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>G6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MIN(K6,1-D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3">
+        <v>344</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.4302325581395349</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-0.08179148995665753</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1/(POWER(B7,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SQRT((D7-POWER(10,-4))*B7*((1-D7+POWER(10,-4))*B7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <v>204</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.357843137254902</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.1541809108412904</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3">
+        <v>136</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.3161764705882353</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.1958475775079571</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.3260869565217391</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.1859370915744533</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.3518518518518519</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.1601721962443405</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.3428571428571429</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.1691669052390495</v>
+      </c>
+      <c r="G12" s="1">
+        <f>1/(POWER(B12,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SQRT((D12-POWER(10,-4))*B12*((1-D12+POWER(10,-4))*B12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K12" s="1">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(K12,1-D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.05882352941176471</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.4532005186844277</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1/(POWER(B13,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f>SQRT((D13-POWER(10,-4))*B13*((1-D13+POWER(10,-4))*B13))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K13" s="1">
+        <f>I13*J13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(K13,1-D13)</f>
         <v>0</v>
       </c>
     </row>
@@ -4665,7 +5955,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4722,7 +6012,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3">
         <v>622</v>
@@ -4765,7 +6055,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3">
         <v>492</v>
@@ -4808,22 +6098,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3">
-        <v>23</v>
+        <v>365</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>0.2173913043478261</v>
+        <v>0.3424657534246575</v>
       </c>
       <c r="E6" s="3">
         <v>0.5120240480961924</v>
       </c>
       <c r="F6" s="1">
-        <v>-0.2946327437483663</v>
+        <v>-0.1695582946715349</v>
       </c>
       <c r="G6" s="1">
         <f>1/(POWER(B6,1.5))</f>
@@ -4851,22 +6141,22 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3">
-        <v>15</v>
+        <v>253</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="3">
-        <v>0.2</v>
+        <v>0.2806324110671937</v>
       </c>
       <c r="E7" s="3">
         <v>0.5120240480961924</v>
       </c>
       <c r="F7" s="1">
-        <v>-0.3120240480961924</v>
+        <v>-0.2313916370289987</v>
       </c>
       <c r="G7" s="1">
         <f>1/(POWER(B7,1.5))</f>
@@ -4894,22 +6184,22 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
       <c r="D8" s="3">
-        <v>0.1</v>
+        <v>0.2754491017964072</v>
       </c>
       <c r="E8" s="3">
         <v>0.5120240480961924</v>
       </c>
       <c r="F8" s="1">
-        <v>-0.4120240480961924</v>
+        <v>-0.2365749462997852</v>
       </c>
       <c r="G8" s="1">
         <f>1/(POWER(B8,1.5))</f>
@@ -4932,6 +6222,350 @@
       </c>
       <c r="L8" s="1">
         <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="3">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.246031746031746</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.2659923020644464</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="3">
+        <v>85</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.1882352941176471</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.3237887539785453</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="3">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.2153846153846154</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.296639432711577</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="3">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.1951219512195122</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.3169020968766802</v>
+      </c>
+      <c r="G12" s="1">
+        <f>1/(POWER(B12,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SQRT((D12-POWER(10,-4))*B12*((1-D12+POWER(10,-4))*B12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K12" s="1">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(K12,1-D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="3">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.1612903225806452</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-0.3507337255155473</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1/(POWER(B13,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f>SQRT((D13-POWER(10,-4))*B13*((1-D13+POWER(10,-4))*B13))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f>G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K13" s="1">
+        <f>I13*J13</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(K13,1-D13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="3">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.2173913043478261</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.2946327437483663</v>
+      </c>
+      <c r="G14" s="1">
+        <f>1/(POWER(B14,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f>SQRT((D14-POWER(10,-4))*B14*((1-D14+POWER(10,-4))*B14))</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f>G14*H14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K14" s="1">
+        <f>I14*J14</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(K14,1-D14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="3">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-0.3120240480961924</v>
+      </c>
+      <c r="G15" s="1">
+        <f>1/(POWER(B15,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SQRT((D15-POWER(10,-4))*B15*((1-D15+POWER(10,-4))*B15))</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f>G15*H15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K15" s="1">
+        <f>I15*J15</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(K15,1-D15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="3">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-0.4120240480961924</v>
+      </c>
+      <c r="G16" s="1">
+        <f>1/(POWER(B16,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SQRT((D16-POWER(10,-4))*B16*((1-D16+POWER(10,-4))*B16))</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <f>G16*H16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K16" s="1">
+        <f>I16*J16</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <f>MIN(K16,1-D16)</f>
         <v>0</v>
       </c>
     </row>
@@ -4943,7 +6577,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5000,7 +6634,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3">
         <v>998</v>
@@ -5043,7 +6677,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B5" s="3">
         <v>683</v>
@@ -5081,6 +6715,307 @@
       </c>
       <c r="L5" s="1">
         <f>MIN(K5,1-D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="3">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.2842105263157895</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.2278135217804029</v>
+      </c>
+      <c r="G6" s="1">
+        <f>1/(POWER(B6,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>G6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MIN(K6,1-D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="3">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.1923076923076923</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-0.3197163557885001</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1/(POWER(B7,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SQRT((D7-POWER(10,-4))*B7*((1-D7+POWER(10,-4))*B7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="3">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.2511544828788011</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="3">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.2263097623819067</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="3">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-0.1483876844598288</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-0.2263097623819067</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-0.1120240480961924</v>
+      </c>
+      <c r="G12" s="1">
+        <f>1/(POWER(B12,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SQRT((D12-POWER(10,-4))*B12*((1-D12+POWER(10,-4))*B12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K12" s="1">
+        <f>I12*J12</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(K12,1-D12)</f>
         <v>0</v>
       </c>
     </row>
@@ -5092,7 +7027,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5149,7 +7084,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>398</v>
@@ -5192,7 +7127,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3">
         <v>157</v>
@@ -5230,6 +7165,178 @@
       </c>
       <c r="L5" s="1">
         <f>MIN(K5,1-D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3">
+        <v>75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-0.1920240480961924</v>
+      </c>
+      <c r="G6" s="1">
+        <f>1/(POWER(B6,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>G6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MIN(K6,1-D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.2558139534883721</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-0.2562100946078203</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1/(POWER(B7,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SQRT((D7-POWER(10,-4))*B7*((1-D7+POWER(10,-4))*B7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-0.3520240480961924</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.1764705882352941</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5120240480961924</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-0.3355534598608982</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>